<commit_message>
json server and comparition
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="212">
   <si>
     <t>Insultos</t>
   </si>
@@ -553,18 +553,6 @@
     <t>Zullenco</t>
   </si>
   <si>
-    <t>Fea</t>
-  </si>
-  <si>
-    <t>fea</t>
-  </si>
-  <si>
-    <t>feo</t>
-  </si>
-  <si>
-    <t>Feo</t>
-  </si>
-  <si>
     <t>Tonto</t>
   </si>
   <si>
@@ -632,6 +620,33 @@
   </si>
   <si>
     <t>Imbecil</t>
+  </si>
+  <si>
+    <t>pendejo</t>
+  </si>
+  <si>
+    <t>pendeja</t>
+  </si>
+  <si>
+    <t>Pendejazo</t>
+  </si>
+  <si>
+    <t>Pendejo</t>
+  </si>
+  <si>
+    <t>puta</t>
+  </si>
+  <si>
+    <t>puto</t>
+  </si>
+  <si>
+    <t>putisimo</t>
+  </si>
+  <si>
+    <t>putisima</t>
+  </si>
+  <si>
+    <t>perra</t>
   </si>
 </sst>
 </file>
@@ -1811,7 +1826,7 @@
       </c>
     </row>
     <row r="185">
-      <c r="A185" s="2" t="s">
+      <c r="A185" s="1" t="s">
         <v>184</v>
       </c>
     </row>
@@ -1821,108 +1836,133 @@
       </c>
     </row>
     <row r="187">
-      <c r="A187" s="2" t="s">
+      <c r="A187" s="1" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="188">
-      <c r="A188" s="2" t="s">
+      <c r="A188" s="1" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="189">
-      <c r="A189" s="2" t="s">
+      <c r="A189" s="1" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="190">
-      <c r="A190" s="2" t="s">
+      <c r="A190" s="1" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="191">
-      <c r="A191" s="2" t="s">
+      <c r="A191" s="1" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="192">
-      <c r="A192" s="2" t="s">
+      <c r="A192" s="1" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="193">
-      <c r="A193" s="2" t="s">
+      <c r="A193" s="1" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="194">
-      <c r="A194" s="2" t="s">
+      <c r="A194" s="1" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="195">
-      <c r="A195" s="2" t="s">
+      <c r="A195" s="1" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="196">
-      <c r="A196" s="2" t="s">
+      <c r="A196" s="1" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="197">
-      <c r="A197" s="2" t="s">
+      <c r="A197" s="1" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="198">
-      <c r="A198" s="2" t="s">
+      <c r="A198" s="1" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="199">
-      <c r="A199" s="2" t="s">
+      <c r="A199" s="1" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="200">
-      <c r="A200" s="2" t="s">
+      <c r="A200" s="1" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="201">
-      <c r="A201" s="2" t="s">
+      <c r="A201" s="1" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="202">
-      <c r="A202" s="2" t="s">
+      <c r="A202" s="1" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="203">
-      <c r="A203" s="2" t="s">
+      <c r="A203" s="1" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="204">
-      <c r="A204" s="2" t="s">
+      <c r="A204" s="1" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="205">
-      <c r="A205" s="2" t="s">
+      <c r="A205" s="1" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="206">
-      <c r="A206" s="2" t="s">
+      <c r="A206" s="1" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="207">
-      <c r="A207" s="2" t="s">
+      <c r="A207" s="1" t="s">
         <v>206</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" s="1" t="s">
+        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>